<commit_message>
Working version of trade statements
</commit_message>
<xml_diff>
--- a/Simplify/Documentation/CapitalGainsCalculationInput.xlsx
+++ b/Simplify/Documentation/CapitalGainsCalculationInput.xlsx
@@ -22,9 +22,6 @@
     <t>S.No.</t>
   </si>
   <si>
-    <t>Name</t>
-  </si>
-  <si>
     <t>Quantity</t>
   </si>
   <si>
@@ -59,6 +56,9 @@
   </si>
   <si>
     <t>Equity Wipro</t>
+  </si>
+  <si>
+    <t>Name1</t>
   </si>
 </sst>
 </file>
@@ -66,7 +66,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="dd\-mmm\-yy"/>
+    <numFmt numFmtId="164" formatCode="dd\-mmm\-yy"/>
   </numFmts>
   <fonts count="3">
     <font>
@@ -114,7 +114,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
@@ -414,7 +414,7 @@
   <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2"/>
@@ -434,22 +434,22 @@
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>4</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>0</v>
@@ -463,7 +463,7 @@
         <v>40156.024943058874</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D2" s="2">
         <v>23222</v>
@@ -486,7 +486,7 @@
         <v>40395.549154925327</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D3" s="2">
         <v>23222</v>
@@ -509,13 +509,13 @@
         <v>40403.326052968485</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D4" s="2">
         <v>23222</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F4" s="4">
         <v>43</v>
@@ -532,13 +532,13 @@
         <v>40666</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D5" s="2">
         <v>3422</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F5" s="4">
         <v>23</v>
@@ -555,13 +555,13 @@
         <v>40666</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D6" s="2">
         <v>3422</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F6" s="4">
         <v>43</v>
@@ -578,7 +578,7 @@
         <v>40729.785615309833</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D7" s="2">
         <v>23222</v>
@@ -601,7 +601,7 @@
         <v>40861.743750263471</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D8" s="2">
         <v>23222</v>
@@ -624,7 +624,7 @@
         <v>41083</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D9" s="2">
         <v>3422</v>
@@ -647,7 +647,7 @@
         <v>41115</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D10" s="2">
         <v>3422</v>
@@ -670,13 +670,13 @@
         <v>41372</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D11" s="2">
         <v>3422</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F11" s="4">
         <v>20</v>
@@ -693,13 +693,13 @@
         <v>41732</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D12" s="2">
         <v>23222</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F12" s="4">
         <v>2.5449999999999999</v>
@@ -717,13 +717,13 @@
         <v>41762</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D13" s="2">
         <v>23222</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F13" s="4">
         <v>2.54</v>
@@ -741,13 +741,13 @@
         <v>41793</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D14" s="2">
         <v>23222</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F14" s="4">
         <v>2.68</v>
@@ -765,13 +765,13 @@
         <v>41823</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D15" s="2">
         <v>23222</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F15" s="4">
         <v>2.54</v>
@@ -789,13 +789,13 @@
         <v>41854</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D16" s="2">
         <v>23222</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F16" s="4">
         <v>2.448</v>
@@ -813,13 +813,13 @@
         <v>41885</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D17" s="2">
         <v>23222</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F17" s="4">
         <v>2.617</v>
@@ -837,13 +837,13 @@
         <v>41915</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D18" s="2">
         <v>23222</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F18" s="4">
         <v>2.722</v>
@@ -861,7 +861,7 @@
         <v>41935</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D19" s="2">
         <v>3422</v>
@@ -885,13 +885,13 @@
         <v>41946</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D20" s="2">
         <v>23222</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F20" s="4">
         <v>2.4929999999999999</v>
@@ -909,13 +909,13 @@
         <v>41976</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D21" s="2">
         <v>23222</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F21" s="4">
         <v>2.5059999999999998</v>
@@ -933,13 +933,13 @@
         <v>42007</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D22" s="2">
         <v>23222</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F22" s="4">
         <v>2.5680000000000001</v>
@@ -957,13 +957,13 @@
         <v>42038</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D23" s="2">
         <v>23222</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F23" s="4">
         <v>2.7170000000000001</v>
@@ -981,13 +981,13 @@
         <v>42066</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D24" s="2">
         <v>23222</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F24" s="4">
         <v>2.504</v>

</xml_diff>

<commit_message>
Fully working - Release candidate
</commit_message>
<xml_diff>
--- a/Simplify/Documentation/CapitalGainsCalculationInput.xlsx
+++ b/Simplify/Documentation/CapitalGainsCalculationInput.xlsx
@@ -58,7 +58,7 @@
     <t>Equity Wipro</t>
   </si>
   <si>
-    <t>Name1</t>
+    <t>Name</t>
   </si>
 </sst>
 </file>
@@ -414,7 +414,7 @@
   <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2"/>

</xml_diff>

<commit_message>
Renamed container statements. Made wipro as closed account in the input excel
</commit_message>
<xml_diff>
--- a/Simplify/Documentation/CapitalGainsCalculationInput.xlsx
+++ b/Simplify/Documentation/CapitalGainsCalculationInput.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="15">
   <si>
     <t>Sale</t>
   </si>
@@ -110,13 +110,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -411,10 +412,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H24"/>
+  <dimension ref="A1:H25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2"/>
@@ -997,6 +998,29 @@
       </c>
       <c r="H24" s="4"/>
     </row>
+    <row r="25" spans="1:8">
+      <c r="A25" s="2">
+        <v>24</v>
+      </c>
+      <c r="B25" s="6">
+        <v>42067</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D25" s="2">
+        <v>3422</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F25" s="4">
+        <v>20</v>
+      </c>
+      <c r="H25">
+        <v>5000</v>
+      </c>
+    </row>
   </sheetData>
   <sortState ref="A2:H24">
     <sortCondition ref="B2:B24"/>

</xml_diff>

<commit_message>
Total profit in summary book
</commit_message>
<xml_diff>
--- a/Simplify/Documentation/CapitalGainsCalculationInput.xlsx
+++ b/Simplify/Documentation/CapitalGainsCalculationInput.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="15">
   <si>
     <t>Sale</t>
   </si>
@@ -412,10 +412,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H25"/>
+  <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2"/>
@@ -1021,6 +1021,29 @@
         <v>5000</v>
       </c>
     </row>
+    <row r="26" spans="1:8">
+      <c r="A26" s="2">
+        <v>35</v>
+      </c>
+      <c r="B26" s="6">
+        <v>42257</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D26" s="2">
+        <v>3422</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F26" s="4">
+        <v>95.88</v>
+      </c>
+      <c r="H26">
+        <v>237900</v>
+      </c>
+    </row>
   </sheetData>
   <sortState ref="A2:H24">
     <sortCondition ref="B2:B24"/>

</xml_diff>